<commit_message>
Add more fields and success message
</commit_message>
<xml_diff>
--- a/data/articulos.xlsx
+++ b/data/articulos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E205"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4324,6 +4324,128 @@
         <v>0</v>
       </c>
     </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>1160</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>bonito</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>4</v>
+      </c>
+      <c r="E206" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>1161</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>masbonito</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>4</v>
+      </c>
+      <c r="E207" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>1162</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>aunmasbonito</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>4</v>
+      </c>
+      <c r="E208" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>1163</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>superbonito</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>4</v>
+      </c>
+      <c r="E209" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>1164</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>superbonito2</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>4</v>
+      </c>
+      <c r="E210" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>1165</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>pepino</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr"/>
+      <c r="D211" t="n">
+        <v>0</v>
+      </c>
+      <c r="E211" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Restricted values and correct refresh
</commit_message>
<xml_diff>
--- a/data/articulos.xlsx
+++ b/data/articulos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4446,6 +4446,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>1166</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>pera</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr"/>
+      <c r="D212" t="n">
+        <v>3</v>
+      </c>
+      <c r="E212" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>1167</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>jmaon</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr"/>
+      <c r="D213" t="n">
+        <v>0</v>
+      </c>
+      <c r="E213" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
forbid delete items and customers when order is in place
</commit_message>
<xml_diff>
--- a/data/articulos.xlsx
+++ b/data/articulos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E213"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4309,28 +4309,32 @@
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>aaa</t>
-        </is>
-      </c>
-      <c r="C205" t="inlineStr"/>
+          <t>bonito</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
       <c r="D205" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E205" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>bonito</t>
+          <t>masbonito</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -4347,11 +4351,11 @@
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>masbonito</t>
+          <t>aunmasbonito</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -4368,11 +4372,11 @@
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>aunmasbonito</t>
+          <t>superbonito</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -4389,11 +4393,11 @@
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>superbonito</t>
+          <t>superbonito2</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -4410,37 +4414,33 @@
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>superbonito2</t>
-        </is>
-      </c>
-      <c r="C210" t="inlineStr">
-        <is>
-          <t>muy bonito</t>
-        </is>
-      </c>
+          <t>pepino</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr"/>
       <c r="D210" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E210" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>pepino</t>
+          <t>pera</t>
         </is>
       </c>
       <c r="C211" t="inlineStr"/>
       <c r="D211" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E211" t="n">
         <v>0</v>
@@ -4448,35 +4448,18 @@
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>pera</t>
+          <t>submit</t>
         </is>
       </c>
       <c r="C212" t="inlineStr"/>
       <c r="D212" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E212" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="n">
-        <v>1167</v>
-      </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>jmaon</t>
-        </is>
-      </c>
-      <c r="C213" t="inlineStr"/>
-      <c r="D213" t="n">
-        <v>0</v>
-      </c>
-      <c r="E213" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
do not allow empty names
</commit_message>
<xml_diff>
--- a/data/articulos.xlsx
+++ b/data/articulos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4446,23 +4446,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212">
-      <c r="A212" t="n">
-        <v>1167</v>
-      </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>submit</t>
-        </is>
-      </c>
-      <c r="C212" t="inlineStr"/>
-      <c r="D212" t="n">
-        <v>0</v>
-      </c>
-      <c r="E212" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
use of google spreadsheets
</commit_message>
<xml_diff>
--- a/data/articulos.xlsx
+++ b/data/articulos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4265,6 +4265,170 @@
         <v>0</v>
       </c>
     </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>1157</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>amigo</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>3</v>
+      </c>
+      <c r="E203" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>1158</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>anonimo</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>3</v>
+      </c>
+      <c r="E204" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>1160</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>bonito</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>4</v>
+      </c>
+      <c r="E205" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>1161</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>masbonito</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>4</v>
+      </c>
+      <c r="E206" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>1162</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>aunmasbonito</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>4</v>
+      </c>
+      <c r="E207" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>1163</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>superbonito</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>4</v>
+      </c>
+      <c r="E208" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>1164</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>superbonito2</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>muy bonito</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>4</v>
+      </c>
+      <c r="E209" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>1165</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>pepino</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr"/>
+      <c r="D210" t="n">
+        <v>0</v>
+      </c>
+      <c r="E210" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>